<commit_message>
Dynamic Programming - Knap Sack and Rod Cutting
</commit_message>
<xml_diff>
--- a/hw1/hw1_data.xlsx
+++ b/hw1/hw1_data.xlsx
@@ -8,32 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevharvell/Desktop/CS/325/hw1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F258543E-A0F2-4543-A3CA-09B0A1E045F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ADC56C-48F8-F64D-A0CC-9401D1E46B46}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{12084929-3E04-7443-9C80-8AC82B018AAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$3:$A$12</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$3:$B$12</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$3:$E$12</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$3:$F$12</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Sheet1!$B$3:$B$12</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Sheet1!$E$3:$E$12</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">Sheet1!$F$2</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Sheet1!$F$3:$F$12</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Sheet1!$A$3:$A$12</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3935,8 +3917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF27EAA-EB7D-E542-936C-085B0B7C9138}">
   <dimension ref="A1:AA995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="151" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>